<commit_message>
cambios de agosto de maydeli
</commit_message>
<xml_diff>
--- a/xlsx/a69_f09UPPachuca.xlsx
+++ b/xlsx/a69_f09UPPachuca.xlsx
@@ -508,9 +508,6 @@
     <t>Francisco I. Madero</t>
   </si>
   <si>
-    <t>http://transparenciadocs.hidalgo.gob.mx/ENTIDADES/UPPachuca7dir1/2022/Abril-Junio/09/Normativa/manual_de_gastos.pdf</t>
-  </si>
-  <si>
     <t>http://transparenciadocs.hidalgo.gob.mx/ENTIDADES/UPPachuca/dir1/2022/Abril-Junio/09/Comprobantes/013-2.pdf</t>
   </si>
   <si>
@@ -659,6 +656,9 @@
   </si>
   <si>
     <t>http://transparenciadocs.hidalgo.gob.mx/ENTIDADES/UPPachuca/dir1/2022/Abril-Junio/09/Informes/037-2.pdf</t>
+  </si>
+  <si>
+    <t>http://transparenciadocs.hidalgo.gob.mx/ENTIDADES/UPPachuca/dir1/2022/Abril-Junio/09/Normativa/manual_de_gastos.pdf</t>
   </si>
 </sst>
 </file>
@@ -1079,7 +1079,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1089,10 +1089,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AE3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E3" sqref="E3"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:C3"/>
+      <selection pane="bottomLeft" activeCell="AF3" sqref="AF3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1635,13 +1635,13 @@
         <v>44656</v>
       </c>
       <c r="AD8" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AE8" s="15">
         <v>13</v>
       </c>
       <c r="AF8" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG8" s="8" t="s">
         <v>114</v>
@@ -1743,13 +1743,13 @@
         <v>44643</v>
       </c>
       <c r="AD9" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AE9" s="15">
         <v>14</v>
       </c>
       <c r="AF9" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG9" s="8" t="s">
         <v>114</v>
@@ -1851,13 +1851,13 @@
         <v>44643</v>
       </c>
       <c r="AD10" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AE10" s="15">
         <v>15</v>
       </c>
       <c r="AF10" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG10" s="8" t="s">
         <v>114</v>
@@ -1959,13 +1959,13 @@
         <v>44643</v>
       </c>
       <c r="AD11" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AE11" s="15">
         <v>16</v>
       </c>
       <c r="AF11" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG11" s="8" t="s">
         <v>114</v>
@@ -2067,13 +2067,13 @@
         <v>44656</v>
       </c>
       <c r="AD12" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AE12" s="15">
         <v>17</v>
       </c>
       <c r="AF12" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG12" s="8" t="s">
         <v>114</v>
@@ -2175,13 +2175,13 @@
         <v>44656</v>
       </c>
       <c r="AD13" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AE13" s="15">
         <v>18</v>
       </c>
       <c r="AF13" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG13" s="8" t="s">
         <v>114</v>
@@ -2283,13 +2283,13 @@
         <v>44657</v>
       </c>
       <c r="AD14" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AE14" s="15">
         <v>19</v>
       </c>
       <c r="AF14" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG14" s="8" t="s">
         <v>114</v>
@@ -2391,13 +2391,13 @@
         <v>44657</v>
       </c>
       <c r="AD15" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AE15" s="15">
         <v>20</v>
       </c>
       <c r="AF15" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG15" s="8" t="s">
         <v>114</v>
@@ -2499,13 +2499,13 @@
         <v>44662</v>
       </c>
       <c r="AD16" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AE16" s="15">
         <v>21</v>
       </c>
       <c r="AF16" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG16" s="8" t="s">
         <v>114</v>
@@ -2607,13 +2607,13 @@
         <v>44662</v>
       </c>
       <c r="AD17" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AE17" s="15">
         <v>22</v>
       </c>
       <c r="AF17" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG17" s="8" t="s">
         <v>114</v>
@@ -2715,13 +2715,13 @@
         <v>44664</v>
       </c>
       <c r="AD18" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AE18" s="15">
         <v>23</v>
       </c>
       <c r="AF18" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG18" s="8" t="s">
         <v>114</v>
@@ -2823,13 +2823,13 @@
         <v>44671</v>
       </c>
       <c r="AD19" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AE19" s="15">
         <v>24</v>
       </c>
       <c r="AF19" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG19" s="8" t="s">
         <v>114</v>
@@ -2931,13 +2931,13 @@
         <v>44667</v>
       </c>
       <c r="AD20" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AE20" s="15">
         <v>25</v>
       </c>
       <c r="AF20" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG20" s="8" t="s">
         <v>114</v>
@@ -3039,13 +3039,13 @@
         <v>44680</v>
       </c>
       <c r="AD21" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AE21" s="15">
         <v>26</v>
       </c>
       <c r="AF21" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG21" s="8" t="s">
         <v>114</v>
@@ -3147,13 +3147,13 @@
         <v>44683</v>
       </c>
       <c r="AD22" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AE22" s="15">
         <v>27</v>
       </c>
       <c r="AF22" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG22" s="8" t="s">
         <v>114</v>
@@ -3255,13 +3255,13 @@
         <v>44706</v>
       </c>
       <c r="AD23" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AE23" s="15">
         <v>28</v>
       </c>
       <c r="AF23" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG23" s="8" t="s">
         <v>114</v>
@@ -3363,13 +3363,13 @@
         <v>44706</v>
       </c>
       <c r="AD24" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AE24" s="15">
         <v>29</v>
       </c>
       <c r="AF24" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG24" s="8" t="s">
         <v>114</v>
@@ -3471,13 +3471,13 @@
         <v>44706</v>
       </c>
       <c r="AD25" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AE25" s="15">
         <v>30</v>
       </c>
       <c r="AF25" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG25" s="8" t="s">
         <v>114</v>
@@ -3579,13 +3579,13 @@
         <v>44707</v>
       </c>
       <c r="AD26" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AE26" s="15">
         <v>31</v>
       </c>
       <c r="AF26" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG26" s="8" t="s">
         <v>114</v>
@@ -3687,13 +3687,13 @@
         <v>44683</v>
       </c>
       <c r="AD27" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AE27" s="15">
         <v>32</v>
       </c>
       <c r="AF27" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG27" s="8" t="s">
         <v>114</v>
@@ -3795,13 +3795,13 @@
         <v>44683</v>
       </c>
       <c r="AD28" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AE28" s="15">
         <v>33</v>
       </c>
       <c r="AF28" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG28" s="8" t="s">
         <v>114</v>
@@ -3903,13 +3903,13 @@
         <v>44818</v>
       </c>
       <c r="AD29" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AE29" s="15">
         <v>34</v>
       </c>
       <c r="AF29" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG29" s="8" t="s">
         <v>114</v>
@@ -4011,13 +4011,13 @@
         <v>44727</v>
       </c>
       <c r="AD30" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AE30" s="15">
         <v>35</v>
       </c>
       <c r="AF30" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG30" s="8" t="s">
         <v>114</v>
@@ -4119,13 +4119,13 @@
         <v>44728</v>
       </c>
       <c r="AD31" s="14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AE31" s="15">
         <v>36</v>
       </c>
       <c r="AF31" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG31" s="8" t="s">
         <v>114</v>
@@ -4227,13 +4227,13 @@
         <v>44732</v>
       </c>
       <c r="AD32" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AE32" s="15">
         <v>37</v>
       </c>
       <c r="AF32" s="14" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="AG32" s="8" t="s">
         <v>114</v>
@@ -4271,31 +4271,31 @@
     <hyperlink ref="AD8" r:id="rId1"/>
     <hyperlink ref="AD22" r:id="rId2"/>
     <hyperlink ref="AD23" r:id="rId3"/>
-    <hyperlink ref="AF10" r:id="rId4"/>
-    <hyperlink ref="AF11:AF32" r:id="rId5" display="http://transparenciadocs.hidalgo.gob.mx/ENTIDADES/UPPachuca7dir1/2022/Abril-Junio/09/Normativa/manual_de_gastos.pdf"/>
-    <hyperlink ref="AF8:AF9" r:id="rId6" display="http://transparenciadocs.hidalgo.gob.mx/ENTIDADES/UPPachuca7dir1/2022/Abril-Junio/09/Normativa/manual_de_gastos.pdf"/>
-    <hyperlink ref="AD9" r:id="rId7"/>
-    <hyperlink ref="AD10" r:id="rId8"/>
-    <hyperlink ref="AD11" r:id="rId9"/>
-    <hyperlink ref="AD12" r:id="rId10"/>
-    <hyperlink ref="AD13" r:id="rId11"/>
-    <hyperlink ref="AD14" r:id="rId12"/>
-    <hyperlink ref="AD15" r:id="rId13"/>
-    <hyperlink ref="AD16" r:id="rId14"/>
-    <hyperlink ref="AD17" r:id="rId15"/>
-    <hyperlink ref="AD18" r:id="rId16"/>
-    <hyperlink ref="AD19" r:id="rId17"/>
-    <hyperlink ref="AD20" r:id="rId18"/>
-    <hyperlink ref="AD21" r:id="rId19"/>
-    <hyperlink ref="AD24" r:id="rId20"/>
-    <hyperlink ref="AD25" r:id="rId21"/>
-    <hyperlink ref="AD26" r:id="rId22"/>
-    <hyperlink ref="AD27" r:id="rId23"/>
-    <hyperlink ref="AD28" r:id="rId24"/>
-    <hyperlink ref="AD29" r:id="rId25"/>
-    <hyperlink ref="AD30" r:id="rId26"/>
-    <hyperlink ref="AD31" r:id="rId27"/>
-    <hyperlink ref="AD32" r:id="rId28"/>
+    <hyperlink ref="AF8:AF9" r:id="rId4" display="http://transparenciadocs.hidalgo.gob.mx/ENTIDADES/UPPachuca7dir1/2022/Abril-Junio/09/Normativa/manual_de_gastos.pdf"/>
+    <hyperlink ref="AD9" r:id="rId5"/>
+    <hyperlink ref="AD10" r:id="rId6"/>
+    <hyperlink ref="AD11" r:id="rId7"/>
+    <hyperlink ref="AD12" r:id="rId8"/>
+    <hyperlink ref="AD13" r:id="rId9"/>
+    <hyperlink ref="AD14" r:id="rId10"/>
+    <hyperlink ref="AD15" r:id="rId11"/>
+    <hyperlink ref="AD16" r:id="rId12"/>
+    <hyperlink ref="AD17" r:id="rId13"/>
+    <hyperlink ref="AD18" r:id="rId14"/>
+    <hyperlink ref="AD19" r:id="rId15"/>
+    <hyperlink ref="AD20" r:id="rId16"/>
+    <hyperlink ref="AD21" r:id="rId17"/>
+    <hyperlink ref="AD24" r:id="rId18"/>
+    <hyperlink ref="AD25" r:id="rId19"/>
+    <hyperlink ref="AD26" r:id="rId20"/>
+    <hyperlink ref="AD27" r:id="rId21"/>
+    <hyperlink ref="AD28" r:id="rId22"/>
+    <hyperlink ref="AD29" r:id="rId23"/>
+    <hyperlink ref="AD30" r:id="rId24"/>
+    <hyperlink ref="AD31" r:id="rId25"/>
+    <hyperlink ref="AD32" r:id="rId26"/>
+    <hyperlink ref="AF8" r:id="rId27"/>
+    <hyperlink ref="AF9:AF32" r:id="rId28" display="http://transparenciadocs.hidalgo.gob.mx/ENTIDADES/UPPachuca7dir1/2022/Abril-Junio/09/Normativa/manual_de_gastos.pdf"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
@@ -4861,7 +4861,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -4869,7 +4869,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -4877,7 +4877,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -4885,7 +4885,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -4893,7 +4893,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -4901,7 +4901,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -4909,7 +4909,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -4917,7 +4917,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -4925,7 +4925,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -4933,7 +4933,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -4941,7 +4941,7 @@
         <v>23</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -4949,7 +4949,7 @@
         <v>24</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -4957,7 +4957,7 @@
         <v>25</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -4965,7 +4965,7 @@
         <v>26</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -4973,7 +4973,7 @@
         <v>27</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -4981,7 +4981,7 @@
         <v>28</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -4989,7 +4989,7 @@
         <v>29</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -4997,7 +4997,7 @@
         <v>30</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -5005,7 +5005,7 @@
         <v>31</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -5013,7 +5013,7 @@
         <v>32</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -5021,7 +5021,7 @@
         <v>33</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -5029,7 +5029,7 @@
         <v>34</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -5037,7 +5037,7 @@
         <v>35</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -5045,7 +5045,7 @@
         <v>36</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -5053,7 +5053,7 @@
         <v>37</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>